<commit_message>
VDX By day Information update
</commit_message>
<xml_diff>
--- a/Bi_Team_Project/Reports/614877.xlsx
+++ b/Bi_Team_Project/Reports/614877.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
   <si>
     <t>Client Name</t>
   </si>
@@ -43,7 +43,7 @@
     <t>Campaign Report date</t>
   </si>
   <si>
-    <t>2018-08-21 to 2018-08-23</t>
+    <t>2018-08-29 to 2018-08-30</t>
   </si>
   <si>
     <t>Agency Name</t>
@@ -115,15 +115,24 @@
     <t>Fullscreen</t>
   </si>
   <si>
-    <t>background</t>
-  </si>
-  <si>
-    <t>visit_site</t>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>find_out_more_tab</t>
   </si>
   <si>
     <t>video_tab</t>
   </si>
   <si>
+    <t>2018-08-29</t>
+  </si>
+  <si>
+    <t>2018-08-30</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
     <t>Live</t>
   </si>
   <si>
@@ -200,15 +209,35 @@
   </si>
   <si>
     <t>Total Interactions</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Impressions</t>
+  </si>
+  <si>
+    <t>Engagements</t>
+  </si>
+  <si>
+    <t>CTR</t>
+  </si>
+  <si>
+    <t>Video Completions</t>
+  </si>
+  <si>
+    <t>Daily Breakdown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0"/>
     <numFmt numFmtId="164" formatCode="#,##0"/>
+    <numFmt numFmtId="164" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -259,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -276,11 +305,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00%"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -321,9 +360,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -698,7 +734,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:N44"/>
+  <dimension ref="B1:N60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
@@ -744,10 +780,10 @@
         <v>7</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="2" customFormat="1">
@@ -766,33 +802,33 @@
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -805,25 +841,25 @@
         <v>15</v>
       </c>
       <c r="C11" s="1">
-        <v>0.02246777163904236</v>
+        <v>0.02825552825552826</v>
       </c>
       <c r="D11" s="1">
-        <v>0.001104972375690608</v>
+        <v>0.001842751842751843</v>
       </c>
       <c r="E11" s="1">
-        <v>0.04918032786885246</v>
+        <v>0.06521739130434782</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G11" s="1">
-        <v>0.1147540983606558</v>
+        <v>0.108695652173913</v>
       </c>
       <c r="H11" s="1">
-        <v>0.1147540983606557</v>
+        <v>0.06521739130434782</v>
       </c>
       <c r="I11" s="1">
-        <v>20.33</v>
+        <v>16.56</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -831,7 +867,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="1">
-        <v>0.003821169277799007</v>
+        <v>0.007562536358347876</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -843,13 +879,13 @@
         <v>17</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="H12" s="1">
-        <v>0.1</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="I12" s="1">
-        <v>7.55</v>
+        <v>9.41</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -857,50 +893,50 @@
         <v>18</v>
       </c>
       <c r="C14" s="1">
-        <v>0.01331582895723931</v>
+        <v>0.01762772632207947</v>
       </c>
       <c r="D14" s="1">
-        <v>0.0005626406601650412</v>
+        <v>0.00089632506722438</v>
       </c>
       <c r="E14" s="1">
-        <v>0.04225352112676056</v>
+        <v>0.05084745762711865</v>
       </c>
       <c r="H14" s="1">
-        <v>0.1126760563380282</v>
+        <v>0.0847457627118644</v>
       </c>
       <c r="I14" s="1">
-        <v>18.53</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="I19" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -913,7 +949,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="1">
-        <v>0.01574803149606299</v>
+        <v>0.009900990099009901</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -928,10 +964,10 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1">
-        <v>7.91</v>
+        <v>6.39</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -939,7 +975,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="1">
-        <v>0.009109311740890687</v>
+        <v>0.0132501948558067</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -951,13 +987,13 @@
         <v>17</v>
       </c>
       <c r="G22" s="1">
-        <v>0</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="H22" s="1">
-        <v>0.05555555555555555</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="I22" s="1">
-        <v>8.109999999999999</v>
+        <v>12.38</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -965,7 +1001,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="1">
-        <v>0.02678571428571428</v>
+        <v>0.05944055944055944</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -977,13 +1013,13 @@
         <v>17</v>
       </c>
       <c r="G23" s="1">
-        <v>0</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="I23" s="1">
-        <v>4.5</v>
+        <v>12.91</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -991,7 +1027,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="1">
-        <v>0.003806416530723219</v>
+        <v>0.002575107296137339</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -1006,10 +1042,10 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>0.1428571428571428</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1">
-        <v>14.1</v>
+        <v>4.91</v>
       </c>
     </row>
     <row r="25" spans="2:9">
@@ -1017,25 +1053,25 @@
         <v>23</v>
       </c>
       <c r="C25" s="1">
-        <v>0.04634581105169341</v>
+        <v>0.06129032258064516</v>
       </c>
       <c r="D25" s="1">
-        <v>0.0053475935828877</v>
+        <v>0.00967741935483871</v>
       </c>
       <c r="E25" s="1">
-        <v>0.1153846153846154</v>
+        <v>0.1578947368421053</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G25" s="1">
-        <v>0.2692307692307692</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="H25" s="1">
-        <v>0.1538461538461539</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="I25" s="1">
-        <v>36.68</v>
+        <v>22.13</v>
       </c>
     </row>
     <row r="27" spans="2:9">
@@ -1043,50 +1079,50 @@
         <v>18</v>
       </c>
       <c r="C27" s="1">
-        <v>0.01331582895723931</v>
+        <v>0.01762772632207947</v>
       </c>
       <c r="D27" s="1">
-        <v>0.0005626406601650412</v>
+        <v>0.00089632506722438</v>
       </c>
       <c r="E27" s="1">
-        <v>0.04225352112676056</v>
+        <v>0.05084745762711865</v>
       </c>
       <c r="H27" s="1">
-        <v>0.1126760563380282</v>
+        <v>0.0847457627118644</v>
       </c>
       <c r="I27" s="1">
-        <v>18.53</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="2:9">
       <c r="B32" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="2:14">
@@ -1102,22 +1138,22 @@
         <v>24</v>
       </c>
       <c r="D34" s="1">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="E34" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F34" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G34" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H34" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I34" s="1">
-        <v>0.1147540983606557</v>
+        <v>0.108695652173913</v>
       </c>
     </row>
     <row r="35" spans="2:14">
@@ -1128,38 +1164,38 @@
         <v>24</v>
       </c>
       <c r="D35" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E35" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F35" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G35" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="1">
-        <v>0</v>
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="39" spans="2:14">
       <c r="B39" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="2:14">
       <c r="C40" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="2:14">
@@ -1200,7 +1236,7 @@
         <v>35</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="2:14">
@@ -1211,16 +1247,16 @@
         <v>0</v>
       </c>
       <c r="D42" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
       </c>
       <c r="G42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="1">
         <v>0</v>
@@ -1232,10 +1268,10 @@
         <v>1</v>
       </c>
       <c r="K42" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" s="1">
         <v>0</v>
@@ -1277,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M43" s="1">
         <v>1</v>
@@ -1340,216 +1376,512 @@
         <v>0</v>
       </c>
     </row>
+    <row r="48" spans="2:14">
+      <c r="B48" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="1">
+        <v>804</v>
+      </c>
+      <c r="E51" s="1">
+        <v>25</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.03109452736318408</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="1">
+        <v>824</v>
+      </c>
+      <c r="E52" s="1">
+        <v>21</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0.02548543689320388</v>
+      </c>
+      <c r="G52" s="1">
+        <v>2</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0.09523809523809523</v>
+      </c>
+      <c r="I52" s="1">
+        <v>5</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0.2380952380952381</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" s="10">
+        <f>sum(D51:D52)</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="10">
+        <f>sum(E51:E52)</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="11">
+        <f>E53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="10">
+        <f>sum(G51:G52)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="11">
+        <f>G53/D53</f>
+        <v>0</v>
+      </c>
+      <c r="I53" s="10">
+        <f>sum(I51:I52)</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="11">
+        <f>I53/D53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="1">
+        <v>882</v>
+      </c>
+      <c r="E56" s="1">
+        <v>7</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0.007936507936507936</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0.1428571428571428</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D57" s="1">
+        <v>837</v>
+      </c>
+      <c r="E57" s="1">
+        <v>6</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0.007168458781362007</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" s="10">
+        <f>sum(D56:D57)</f>
+        <v>0</v>
+      </c>
+      <c r="E58" s="10">
+        <f>sum(E56:E57)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="11">
+        <f>E58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="10">
+        <f>sum(G56:G57)</f>
+        <v>0</v>
+      </c>
+      <c r="H58" s="11">
+        <f>G58/D58</f>
+        <v>0</v>
+      </c>
+      <c r="I58" s="10">
+        <f>sum(I56:I57)</f>
+        <v>0</v>
+      </c>
+      <c r="J58" s="11">
+        <f>I58/D58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="B60" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:R5">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="13">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="14">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:H14">
-    <cfRule type="containsBlanks" dxfId="2" priority="10">
+    <cfRule type="containsBlanks" dxfId="4" priority="22">
       <formula>LEN(TRIM(B14))=0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="23">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:I18">
-    <cfRule type="containsBlanks" dxfId="1" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="16">
       <formula>LEN(TRIM(B18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:H27">
-    <cfRule type="containsBlanks" dxfId="2" priority="13">
+    <cfRule type="containsBlanks" dxfId="4" priority="25">
       <formula>LEN(TRIM(B27))=0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="26">
       <formula>LEN(TRIM(B27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:I31">
-    <cfRule type="containsBlanks" dxfId="1" priority="5">
+    <cfRule type="containsBlanks" dxfId="3" priority="17">
       <formula>LEN(TRIM(B31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40:N40">
-    <cfRule type="containsBlanks" dxfId="1" priority="6">
+    <cfRule type="containsBlanks" dxfId="3" priority="18">
       <formula>LEN(TRIM(B40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:N41">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="20">
       <formula>LEN(TRIM(B41))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="9">
+    <cfRule type="containsBlanks" dxfId="2" priority="21">
       <formula>LEN(TRIM(B41))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B48:J48">
+    <cfRule type="containsBlanks" dxfId="3" priority="57">
+      <formula>LEN(TRIM(B48))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B8:I8">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="15">
       <formula>LEN(TRIM(B8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="28">
       <formula>LEN(TRIM(C11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="34">
       <formula>LEN(TRIM(C21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:N39">
-    <cfRule type="containsBlanks" dxfId="1" priority="7">
+    <cfRule type="containsBlanks" dxfId="3" priority="19">
       <formula>LEN(TRIM(C39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="34">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="46">
       <formula>LEN(TRIM(C43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D12">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="29">
       <formula>LEN(TRIM(D11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="35">
       <formula>LEN(TRIM(D21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:D36">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="28">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="40">
       <formula>LEN(TRIM(D34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="35">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="47">
       <formula>LEN(TRIM(D43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D51:E53">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(D51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56:E58">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="7">
+      <formula>LEN(TRIM(D56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E11:E12">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="30">
       <formula>LEN(TRIM(E11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21:E25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="24">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="36">
       <formula>LEN(TRIM(E21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E36">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="29">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="41">
       <formula>LEN(TRIM(E34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43:E44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="36">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="48">
       <formula>LEN(TRIM(E43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F12">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="31">
       <formula>LEN(TRIM(F11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:F25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="37">
       <formula>LEN(TRIM(F21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:F36">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="30">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="42">
       <formula>LEN(TRIM(F34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:F44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="37">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="49">
       <formula>LEN(TRIM(F43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F51:F53">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(F51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F56:F58">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="8">
+      <formula>LEN(TRIM(F56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G11:G12">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="32">
       <formula>LEN(TRIM(G11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:G25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="38">
       <formula>LEN(TRIM(G21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:G36">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="31">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="43">
       <formula>LEN(TRIM(G34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="50">
       <formula>LEN(TRIM(G43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G51:G53">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="3">
+      <formula>LEN(TRIM(G51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56:G58">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="9">
+      <formula>LEN(TRIM(G56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H11:H12">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="33">
       <formula>LEN(TRIM(H11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21:H25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="39">
       <formula>LEN(TRIM(H21))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34:H36">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="32">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="44">
       <formula>LEN(TRIM(H34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="51">
       <formula>LEN(TRIM(H43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H51:H53">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="4">
+      <formula>LEN(TRIM(H51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H56:H58">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="10">
+      <formula>LEN(TRIM(H56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="24">
       <formula>LEN(TRIM(I14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="27">
       <formula>LEN(TRIM(I27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:I36">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="33">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="45">
       <formula>LEN(TRIM(I34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:I44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="40">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="52">
       <formula>LEN(TRIM(I43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I51:I53">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+      <formula>LEN(TRIM(I51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I56:I58">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="11">
+      <formula>LEN(TRIM(I56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J43:J44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="41">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="53">
       <formula>LEN(TRIM(J43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J51:J53">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="6">
+      <formula>LEN(TRIM(J51))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J56:J58">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="12">
+      <formula>LEN(TRIM(J56))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K43:K44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="42">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="54">
       <formula>LEN(TRIM(K43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43:L44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="43">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="55">
       <formula>LEN(TRIM(L43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M43:M44">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="56">
       <formula>LEN(TRIM(M43))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>